<commit_message>
update sample information to result v4
</commit_message>
<xml_diff>
--- a/v4/v4_standard/std_random-wo-gaussianProj/random_init_wo_gaussianProj_regression.xlsx
+++ b/v4/v4_standard/std_random-wo-gaussianProj/random_init_wo_gaussianProj_regression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v4\v4_standard\std_random-wo-gaussianProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDBB39F-416E-4493-A33B-4471918C0253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02045E18-C8BC-4EF9-A87F-3859A75CFCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="957">
   <si>
     <t>dataname:task_type</t>
   </si>
@@ -2829,12 +2829,81 @@
   <si>
     <t>diamonds:regression</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean of std</t>
+  </si>
+  <si>
+    <t>std of mean</t>
+  </si>
+  <si>
+    <t>mean_distance_correlation</t>
+  </si>
+  <si>
+    <t>datasets</t>
+  </si>
+  <si>
+    <t>abalone</t>
+  </si>
+  <si>
+    <t>airfoil_self_noise</t>
+  </si>
+  <si>
+    <t>Brazilian_houses</t>
+  </si>
+  <si>
+    <t>california_housing</t>
+  </si>
+  <si>
+    <t>colleges</t>
+  </si>
+  <si>
+    <t>combined_cycle_power_plant</t>
+  </si>
+  <si>
+    <t>concrete_compressive_strength</t>
+  </si>
+  <si>
+    <t>diamonds</t>
+  </si>
+  <si>
+    <t>elevators</t>
+  </si>
+  <si>
+    <t>House_16H</t>
+  </si>
+  <si>
+    <t>house_sales</t>
+  </si>
+  <si>
+    <t>OnlineNewsPopularity</t>
+  </si>
+  <si>
+    <t>physicochemical_properties_of_protein_tertiary_structure</t>
+  </si>
+  <si>
+    <t>pol</t>
+  </si>
+  <si>
+    <t>qsar_aquatic_toxicity</t>
+  </si>
+  <si>
+    <t>qsar_fish_toxicity</t>
+  </si>
+  <si>
+    <t>yacht_hydrodynamics</t>
+  </si>
+  <si>
+    <t>superconductivty_data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2847,18 +2916,21 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2917,7 +2989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2930,6 +3002,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3232,21 +3305,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K138" sqref="K138:N138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="28.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3274,8 +3347,20 @@
       <c r="I1" s="1" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3303,8 +3388,20 @@
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>939</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.98345470428466797</v>
+      </c>
+      <c r="M2" s="8">
+        <v>0.34772807359695429</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0.71116379329136437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3333,7 +3430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3362,7 +3459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3391,7 +3488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3420,7 +3517,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3449,7 +3546,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3478,7 +3575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3507,7 +3604,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>931</v>
       </c>
@@ -3535,8 +3632,20 @@
       <c r="I10" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>940</v>
+      </c>
+      <c r="L10" s="8">
+        <v>1.6599069833755491</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0.31834891438484192</v>
+      </c>
+      <c r="N10" s="8">
+        <v>7.5102585554122928E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3565,7 +3674,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3594,7 +3703,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3623,7 +3732,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3652,7 +3761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3681,7 +3790,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3710,7 +3819,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3739,7 +3848,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>933</v>
       </c>
@@ -3767,8 +3876,20 @@
       <c r="I18" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>941</v>
+      </c>
+      <c r="L18" s="8">
+        <v>2.5506405830383301</v>
+      </c>
+      <c r="M18" s="8">
+        <v>3.9748160839080811</v>
+      </c>
+      <c r="N18" s="8">
+        <v>0.12592234756007339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3797,7 +3918,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3826,7 +3947,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3855,7 +3976,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3884,7 +4005,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3913,7 +4034,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3942,7 +4063,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3971,7 +4092,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>172</v>
       </c>
@@ -3999,8 +4120,20 @@
       <c r="I26" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>942</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1.00010466575623</v>
+      </c>
+      <c r="M26" s="8">
+        <v>2.952026436105371E-3</v>
+      </c>
+      <c r="N26" s="8">
+        <v>5.5523519005094259E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4029,7 +4162,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -4058,7 +4191,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -4087,7 +4220,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -4116,7 +4249,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -4145,7 +4278,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4307,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -4203,7 +4336,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>224</v>
       </c>
@@ -4231,8 +4364,20 @@
       <c r="I34" s="6" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>943</v>
+      </c>
+      <c r="L34" s="8">
+        <v>132.117919921875</v>
+      </c>
+      <c r="M34" s="8">
+        <v>780.28363037109398</v>
+      </c>
+      <c r="N34" s="8">
+        <v>0.1290543350657305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4261,7 +4406,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4290,7 +4435,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -4319,7 +4464,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -4348,7 +4493,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4377,7 +4522,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -4406,7 +4551,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4435,7 +4580,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>277</v>
       </c>
@@ -4463,8 +4608,20 @@
       <c r="I42" s="5" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>944</v>
+      </c>
+      <c r="L42" s="8">
+        <v>1.0054241418838501</v>
+      </c>
+      <c r="M42" s="8">
+        <v>3.7787000183016062E-3</v>
+      </c>
+      <c r="N42" s="8">
+        <v>0.22805456320444739</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4493,7 +4650,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4522,7 +4679,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4551,7 +4708,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4580,7 +4737,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -4609,7 +4766,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4638,7 +4795,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -4667,7 +4824,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>328</v>
       </c>
@@ -4695,8 +4852,20 @@
       <c r="I50" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>945</v>
+      </c>
+      <c r="L50" s="8">
+        <v>1.7419309616088869</v>
+      </c>
+      <c r="M50" s="8">
+        <v>0.95711261034011841</v>
+      </c>
+      <c r="N50" s="8">
+        <v>5.5853222097669332E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -4725,7 +4894,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4754,7 +4923,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -4783,7 +4952,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -4812,7 +4981,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -4841,7 +5010,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -4870,7 +5039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -4899,7 +5068,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>934</v>
       </c>
@@ -4927,8 +5096,20 @@
       <c r="I58" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>946</v>
+      </c>
+      <c r="L58" s="8">
+        <v>1.1640166044235229</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1.452937960624695</v>
+      </c>
+      <c r="N58" s="8">
+        <v>0.18491559558444551</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -4957,7 +5138,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -4986,7 +5167,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -5015,7 +5196,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -5044,7 +5225,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -5073,7 +5254,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -5102,7 +5283,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -5131,7 +5312,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>428</v>
       </c>
@@ -5159,8 +5340,20 @@
       <c r="I66" s="2" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>947</v>
+      </c>
+      <c r="L66" s="8">
+        <v>0.87084829807281494</v>
+      </c>
+      <c r="M66" s="8">
+        <v>1.6319278478622441</v>
+      </c>
+      <c r="N66" s="8">
+        <v>0.1184010723837061</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -5189,7 +5382,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -5218,7 +5411,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -5247,7 +5440,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -5276,7 +5469,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -5305,7 +5498,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -5334,7 +5527,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5556,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>475</v>
       </c>
@@ -5391,8 +5584,20 @@
       <c r="I74" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>948</v>
+      </c>
+      <c r="L74" s="8">
+        <v>1.7806739807128911</v>
+      </c>
+      <c r="M74" s="8">
+        <v>0.85412532091140747</v>
+      </c>
+      <c r="N74" s="8">
+        <v>8.4788465499877924E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5626,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -5450,7 +5655,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -5479,7 +5684,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -5508,7 +5713,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -5537,7 +5742,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -5566,7 +5771,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -5595,7 +5800,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>524</v>
       </c>
@@ -5623,8 +5828,20 @@
       <c r="I82" s="2" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K82" t="s">
+        <v>949</v>
+      </c>
+      <c r="L82" s="8">
+        <v>2.0755412578582759</v>
+      </c>
+      <c r="M82" s="8">
+        <v>7.7008585929870614</v>
+      </c>
+      <c r="N82" s="8">
+        <v>5.8548667214133522E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -5653,7 +5870,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -5682,7 +5899,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -5711,7 +5928,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -5740,7 +5957,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -5769,7 +5986,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -5798,7 +6015,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -5827,7 +6044,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>932</v>
       </c>
@@ -5855,8 +6072,20 @@
       <c r="I90" s="2" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K90" t="s">
+        <v>950</v>
+      </c>
+      <c r="L90" s="8">
+        <v>2.1313338279724121</v>
+      </c>
+      <c r="M90" s="8">
+        <v>1.844881534576416</v>
+      </c>
+      <c r="N90" s="8">
+        <v>3.617335952417243E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -5885,7 +6114,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -5914,7 +6143,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -5943,7 +6172,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -5972,7 +6201,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -6001,7 +6230,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -6030,7 +6259,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -6059,7 +6288,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>621</v>
       </c>
@@ -6087,8 +6316,20 @@
       <c r="I98" s="3" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K98" t="s">
+        <v>951</v>
+      </c>
+      <c r="L98" s="8">
+        <v>0.99856197834014893</v>
+      </c>
+      <c r="M98" s="8">
+        <v>6.3572605140507221E-3</v>
+      </c>
+      <c r="N98" s="8">
+        <v>0.54962857564290368</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -6117,7 +6358,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -6146,7 +6387,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -6175,7 +6416,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -6204,7 +6445,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -6233,7 +6474,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -6262,7 +6503,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>12</v>
       </c>
@@ -6291,7 +6532,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>669</v>
       </c>
@@ -6319,8 +6560,20 @@
       <c r="I106" s="5" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K106" t="s">
+        <v>952</v>
+      </c>
+      <c r="L106" s="8">
+        <v>1.110600352287292</v>
+      </c>
+      <c r="M106" s="8">
+        <v>1.993265748023987</v>
+      </c>
+      <c r="N106" s="8">
+        <v>1.027935278331134E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>12</v>
       </c>
@@ -6349,7 +6602,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -6378,7 +6631,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -6407,7 +6660,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -6436,7 +6689,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -6465,7 +6718,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -6494,7 +6747,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -6523,7 +6776,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>718</v>
       </c>
@@ -6551,8 +6804,20 @@
       <c r="I114" s="3" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K114" t="s">
+        <v>953</v>
+      </c>
+      <c r="L114" s="8">
+        <v>2.0983693599700932</v>
+      </c>
+      <c r="M114" s="8">
+        <v>1.2690484523773189</v>
+      </c>
+      <c r="N114" s="8">
+        <v>0.14052917276109969</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>12</v>
       </c>
@@ -6581,7 +6846,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>12</v>
       </c>
@@ -6610,7 +6875,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>12</v>
       </c>
@@ -6639,7 +6904,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>12</v>
       </c>
@@ -6668,7 +6933,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>12</v>
       </c>
@@ -6697,7 +6962,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>12</v>
       </c>
@@ -6726,7 +6991,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>12</v>
       </c>
@@ -6755,7 +7020,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>769</v>
       </c>
@@ -6783,8 +7048,20 @@
       <c r="I122" s="2" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K122" t="s">
+        <v>954</v>
+      </c>
+      <c r="L122" s="8">
+        <v>1.6366721391677861</v>
+      </c>
+      <c r="M122" s="8">
+        <v>1.7532403469085689</v>
+      </c>
+      <c r="N122" s="8">
+        <v>3.9728323618570961E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -6813,7 +7090,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>12</v>
       </c>
@@ -6842,7 +7119,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>12</v>
       </c>
@@ -6871,7 +7148,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>12</v>
       </c>
@@ -6900,7 +7177,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -6929,7 +7206,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>12</v>
       </c>
@@ -6958,7 +7235,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
         <v>12</v>
       </c>
@@ -6987,7 +7264,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
         <v>819</v>
       </c>
@@ -7015,8 +7292,20 @@
       <c r="I130" s="5" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K130" t="s">
+        <v>955</v>
+      </c>
+      <c r="L130" s="8">
+        <v>1.732479929924011</v>
+      </c>
+      <c r="M130" s="8">
+        <v>0.29961645603179932</v>
+      </c>
+      <c r="N130" s="8">
+        <v>6.6571203867594395E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -7045,7 +7334,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
         <v>12</v>
       </c>
@@ -7074,7 +7363,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>12</v>
       </c>
@@ -7103,7 +7392,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -7132,7 +7421,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -7161,7 +7450,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
         <v>12</v>
       </c>
@@ -7190,7 +7479,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
         <v>12</v>
       </c>
@@ -7219,7 +7508,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
         <v>868</v>
       </c>
@@ -7247,8 +7536,20 @@
       <c r="I138" s="6" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K138" t="s">
+        <v>956</v>
+      </c>
+      <c r="L138" s="8">
+        <v>1.0917073488235469</v>
+      </c>
+      <c r="M138" s="8">
+        <v>4.0277112275362008E-2</v>
+      </c>
+      <c r="N138" s="8">
+        <v>0.16603826828944829</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -7277,7 +7578,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -7306,7 +7607,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -7335,7 +7636,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
         <v>12</v>
       </c>
@@ -7364,7 +7665,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
         <v>12</v>
       </c>
@@ -7393,7 +7694,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>12</v>
       </c>
@@ -7422,7 +7723,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>12</v>
       </c>
@@ -7451,7 +7752,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -7480,7 +7781,7 @@
         <v>3.9629629629629628</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>12</v>
       </c>

</xml_diff>